<commit_message>
added source data and correct composition text
</commit_message>
<xml_diff>
--- a/ePICreator/Mirtazapine.xlsx
+++ b/ePICreator/Mirtazapine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/vulcan-eproduct-info/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D169C9-C941-684F-8646-88BF6C6C7127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C69A2D3-7614-BF4F-BA9E-107F54BA101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="9" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="9" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="146">
   <si>
     <t>id</t>
   </si>
@@ -306,416 +306,27 @@
     <t>package_leaflet</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;p&gt;Karvea 75 mg tablets&lt;/p&gt;
-            &lt;p&gt;irbesartan&lt;/p&gt;
-            &lt;b&gt;Read all of this leaflet carefully before you start taking this medicine because it contains important information for you.&lt;/b&gt;
-            &lt;ul&gt;
-                &lt;li&gt;Keep this leaflet. You may need to read it again.&lt;/li&gt;
-                &lt;li&gt;If you have any further questions, ask your doctor or pharmacist.&lt;/li&gt;
-                &lt;li&gt;This medicine has been prescribed for you only. Do not pass it on to others. It may harm them, even if their signs of illness are the same as yours.&lt;/li&gt;
-                &lt;li&gt;If you get any side effects, talk to your doctor or pharmacist. This includes any possible side effects not listed in this leaflet. See section 4.&lt;/li&gt;
-            &lt;/ul&gt;
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>what_in_leaflet</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;ul&gt;
-                &lt;li&gt;What Karvea is and what it is used for&lt;/li&gt;
-                &lt;li&gt;What you need to know before you take Karvea&lt;/li&gt;
-                &lt;li&gt;How to take Karvea&lt;/li&gt;
-                &lt;li&gt;Possible side effects&lt;/li&gt;
-                &lt;li&gt;How to store Karvea&lt;/li&gt;
-                &lt;li&gt;Contents of the pack and other information&lt;/li&gt;
-            &lt;/ul&gt;
-        &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;p&gt;
-                Karvea belongs to a group of medicines known as angiotensin-II receptor antagonists. Angiotensin-II is a substance produced in the body which binds to receptors in blood vessels causing them to tighten. This results in an increase in blood pressure. Karvea prevents the binding of angiotensin-II to these receptors, causing the blood vessels to relax and the blood pressure to lower. Karvea slows the decrease of kidney function in patients with high blood pressure and type 2 diabetes.
-            &lt;/p&gt;
-            &lt;p&gt;Karvea is used in adult patients&lt;/p&gt;
-            &lt;ul&gt;
-                &lt;li&gt;to treat high blood pressure (essential hypertension)&lt;/li&gt;
-                &lt;li&gt;to protect the kidney in patients with high blood pressure, type 2 diabetes and laboratory
-                    evidence of impaired kidney function.&lt;/li&gt;
-            &lt;/ul&gt;
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>what_product_is</t>
   </si>
   <si>
     <t>before_take</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;b&gt;Do not take Karvea&lt;/b&gt;
-            &lt;ul&gt;
-                &lt;li&gt;if you are allergic to irbesartan or any other ingredients of this medicine (listed in section 6)&lt;/li&gt;
-                &lt;li&gt;if you are more than 3 months pregnant. (It is also better to avoid Karvea in early pregnancy –
-                    see pregnancy section)&lt;/li&gt;
-                &lt;li&gt;&lt;b&gt;if you have diabetes or impaired kidney function&lt;/b&gt; and you are treated with a blood pressure
-                    lowering medicine containing aliskiren.&lt;/li&gt;
-            &lt;/ul&gt;
-            &lt;b&gt;Warning and precautions&lt;/b&gt;
-            &lt;p&gt;Talk to your doctor before taking Karvea and &lt;b&gt;if any of the following apply to you:&lt;/b&gt;&lt;/p&gt;
-            &lt;ul&gt;
-                &lt;li&gt;if you get excessive vomiting or diarrhoea&lt;/li&gt;
-                &lt;li&gt;if you suffer from kidney problems&lt;/li&gt;
-                &lt;li&gt;if you suffer from heart problems&lt;/li&gt;
-                &lt;li&gt;if you receive Karvea for diabetic kidney disease. In this case your doctor may perform regular
-                    blood tests, especially for measuring blood potassium levels in case of poor kidney function&lt;/li&gt;
-                &lt;li&gt;if you develop low blood sugar levels (symptoms may include sweating, weakness, hunger,
-                    dizziness, trembling, headache, flushing or paleness, numbness, having a fast, pounding heart
-                    beat), particularly if you are being treated for diabetes.&lt;/li&gt;
-                &lt;li&gt;if you are going to have an operation (surgery) or be given anaesthetics&lt;/li&gt;
-                &lt;li&gt;
-                    &lt;ul&gt;
-                        &lt;li&gt;an ACE-inhibitor (for example enalapril, lisinopril, ramipril), in particular if you have diabetes-related kidney problems.&lt;/li&gt;
-                        &lt;li&gt;aliskiren&lt;/li&gt;
-                    &lt;/ul&gt;
-                &lt;/li&gt;
-            &lt;/ul&gt;
-            &lt;p&gt;Your doctor may check your kidney function, blood pressure, and the amount of electrolytes (e.g. potassium) in your blood at regular intervals.&lt;/p&gt;
-            &lt;p&gt;See also information under the heading “Do not take Karvea”.&lt;/p&gt;
-            &lt;p&gt;You must tell your doctor if you think you are (or might become) pregnant. Karvea is not recommended in early pregnancy, and must not be taken if you are more than 3 months pregnant, as it may cause serious harm to your baby if used at that stage (see pregnancy section).&lt;/p&gt;
-            &lt;b&gt;Children and adolescents&lt;/b&gt;
-            &lt;p&gt;This medicinal product should not be used in children and adolescents because the safety and efficacy have not yet been fully established.&lt;/p&gt;
-            &lt;b&gt;Other medicines and Karvea&lt;/b&gt;
-            &lt;p&gt;Tell your doctor or pharmacist if you are taking, have recently taken or might take any other medicines.&lt;/p&gt;
-            &lt;p&gt;Your doctor may need to change your dose and/or to take other precautions:
-                If you are taking an ACE-inhibitor or aliskiren (see also information under the headings “Do not take
-                Karvea” and “Warnings and precautions”).&lt;/p&gt;
-            &lt;b&gt;You may need to have blood checks if you take:&lt;/b&gt;
-            &lt;ul&gt;
-                &lt;li&gt;potassium supplements&lt;/li&gt;
-                &lt;li&gt;salt substitutes containing potassium&lt;/li&gt;
-                &lt;li&gt;potassium-sparing medicines (such as certain diuretics)&lt;/li&gt;
-                &lt;li&gt;medicines containing lithium&lt;/li&gt;
-                &lt;li&gt;repaglinide (medication used for lowering blood sugar levels)&lt;/li&gt;
-            &lt;/ul&gt;
-            &lt;p&gt;If you take certain painkillers, called non-steroidal anti-inflammatory drugs, the effect of irbesartan may be reduced.&lt;/p&gt;
-            &lt;b&gt;Karvea with food and drink&lt;/b&gt;
-            &lt;p&gt;Karvea can be taken with or without food.&lt;/p&gt;
-            &lt;b&gt;Pregnancy and breast-feeding&lt;/b&gt;
-            &lt;b&gt;Pregnancy&lt;/b&gt;
-            &lt;p&gt;You must tell your doctor if you think you are (or might become) pregnant. Your doctor will normally advise you to stop taking Karvea before you become pregnant or as soon as you know you are pregnant and will advise you to take another medicine instead of Karvea. Karvea is not recommended in early pregnancy, and must not be taken when more than 3 months pregnant, as it may cause serious harm to your baby if used after the third month of pregnancy.&lt;/p&gt;
-            &lt;b&gt;Breast-feeding&lt;/b&gt;
-            &lt;p&gt;Tell your doctor if you are breast-feeding or about to start breast-feeding. Karvea is not recommended for mothers who are breast-feeding, and your doctor may choose another treatment for you if you wish to breast-feed, especially if your baby is newborn, or was born prematurely.&lt;/p&gt;
-            &lt;b&gt;Driving and using machines&lt;/b&gt;
-            &lt;p&gt;Karvea is unlikely to affect your ability to drive or use machines. However, occasionally dizziness or weariness may occur during treatment of high blood pressure. If you experience these, talk to your doctor before attempting to drive or use machines.
-            &lt;/p&gt;
-            &lt;b&gt;Karvea contains lactose.&lt;/b&gt;
-            &lt;p&gt;If you have been told by your doctor that you have an intolerance to some sugars (e.g. lactose), contact your doctor before taking this medicinal product.&lt;/p&gt;
-            &lt;b&gt;Karvea contains sodium.&lt;/b&gt;
-            &lt;p&gt;This medicine contains less than 1 mmol sodium (23 mg) per tablet, that is to say essentially ‘sodium-free’.&lt;/p&gt;            
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>how_to_take</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;b&gt;Always take this medicine exactly as your doctor has told you. Check with your doctor or pharmacist if you are not sure.&lt;/b&gt;
-            &lt;b&gt;Method of administration&lt;/b&gt;
-            &lt;p&gt;Karvea is for oral use. Swallow the tablets with a sufficient amount of fluid (e.g. one glass of water). You can take Karvea with or without food. Try to take your daily dose at about the same time each day. It is important that you continue to take Karvea until your doctor tells you otherwise.&lt;/p&gt;
-            &lt;ul&gt;
-                &lt;li&gt;
-                    &lt;b&gt;Patients with high blood pressure&lt;/b&gt;
-                    &lt;p&gt;The usual dose is 150 mg once a day (two tablets a day). The dose may later be increased to 300 mg (four tablets a day) once daily depending on blood pressure response.&lt;/p&gt;
-                &lt;/li&gt;
-                &lt;li&gt;
-                    &lt;b&gt;Patients with high blood pressure and type 2 diabetes with kidney disease&lt;/b&gt;
-                    &lt;p&gt;In patients with high blood pressure and type 2 diabetes, 300 mg (four tablets a day) once daily is the preferred maintenance dose for the treatment of associated kidney disease.&lt;/p&gt;
-                &lt;/li&gt;
-            &lt;/ul&gt;
-            &lt;p&gt;The doctor may advise a lower dose, especially when starting treatment in certain patients such as those on haemodialysis, or those over the age of 75 years.
-            &lt;/p&gt;
-            &lt;p&gt;The maximal blood pressure lowering effect should be reached 4-6 weeks after beginning treatment.&lt;/p&gt;
-            &lt;b&gt;Use in children and adolescents&lt;/b&gt;
-            &lt;p&gt;Karvea should not be given to children under 18 years of age. If a child swallows some tablets, contact your doctor immediately.&lt;/p&gt;
-            &lt;b&gt;If you take more Karvea than you should&lt;/b&gt;
-            &lt;p&gt;If you accidentally take too many tablets, contact your doctor immediately.&lt;/p&gt;
-            &lt;b&gt;If you forget to take Karvea&lt;/b&gt;
-            &lt;p&gt;If you accidentally miss a daily dose, just take the next dose as normal. Do not take a double dose to make up for a forgotten dose.&lt;/p&gt;
-            &lt;p&gt;If you have any further questions on the use of this medicine, ask your doctor or pharmacist.&lt;/p&gt;     
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>side_effects</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;p&gt;Like all medicines, this medicine can cause side effects, although not everybody gets them. Some of these effects may be serious and may require medical attention.&lt;/p&gt;
-            &lt;p&gt;As with similar medicines, rare cases of allergic skin reactions (rash, urticaria), as well as localised swelling of the face, lips and/or tongue have been reported in patients taking irbesartan. If you get any of these symptoms or get short of breath, stop taking Karvea and contact your doctor immediately.&lt;/p&gt;
-            &lt;p&gt;The frequency of the side effects listed below is defined using the following convention:&lt;/p&gt;
-            &lt;p&gt;Very common: may affect more than 1 in 10 people&lt;/p&gt;
-            &lt;p&gt;Common: may affect up to 1 in 10 people&lt;/p&gt;
-            &lt;p&gt;Uncommon: may affect up to 1 in 100 people&lt;/p&gt;
-            &lt;p&gt;Side effects reported in clinical studies for patients treated with Karvea were:&lt;/p&gt;
-            &lt;ul&gt;
-                &lt;li&gt;Very common (may affect more than 1 in 10 people): if you suffer from high blood pressure and
-                    type 2 diabetes with kidney disease, blood tests may show an increased level of potassium.&lt;/li&gt;
-                &lt;li&gt;Common (may affect up to 1 10 people): dizziness, feeling sick/vomiting, fatigue and blood tests may show raised levels of an enzyme that measures the muscle and heart function (creatine kinase enzyme). In patients with high blood pressure and type 2 diabetes with kidney disease, dizziness when getting up from a lying or sitting position, low blood pressure when getting up from a lying or sitting position, pain in joints or muscles and decreased levels of a protein in the red blood cells (haemoglobin) were also reported.
-                &lt;/li&gt;
-                &lt;li&gt;Uncommon (may affect up to 1 in 100 people): heart rate increased, flushing, cough, diarrhoea, indigestion/heartburn, sexual dysfunction (problems with sexual performance), chest pain.&lt;/li&gt;
-            &lt;/ul&gt;
-            &lt;p&gt;Some undesirable effects have been reported since marketing of Karvea. Undesirable effects where the frequency is not known are: feeling of spinning, headache, taste disturbance, ringing in the ears, muscle cramps, pain in joints and muscles, decreased number of red blood cells (anaemia – symptoms may include tiredness, headaches, being short of breath when exercising, dizziness and looking pale), reduced number of platelets, abnormal liver function, increased blood potassium levels, impaired kidney function, inflammation of small blood vessels mainly affecting the skin (a condition known as leukocytoclastic vasculitis), severe allergic reactions (anaphylactic shock) and low blood sugar levels. Uncommon cases of jaundice (yellowing of the skin and/or whites of the eyes) have also been reported.
-            &lt;/p&gt;
-            &lt;b&gt;Reporting of side effects&lt;/b&gt;
-            &lt;p&gt;If you get any side effects, talk to your doctor or pharmacist. This includes any possible side effects not listed in this leaflet. You can also report side effects directly via the national reporting system listed in Appendix V. By reporting side effects you can help provide more information on the safety of this medicine.
-            &lt;/p&gt;
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>how_to_store</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;p&gt;Keep this medicine out of the sight and reach of children.&lt;/p&gt;
-            &lt;p&gt;
-                Do not use this medicine after the expiry date which is stated on the carton and on the blister after EXP. The expiry date refers to the last day of that month.
-            &lt;/p&gt;
-            &lt;p&gt;Do not store above 30°C.&lt;/p&gt;
-            &lt;p&gt;Do not throw away any medicines via wastewater or household waste. Ask your pharmacist how to throw away of medicines you no longer use. These measures will help protect the environment.
-            &lt;/p&gt;
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>other_info</t>
   </si>
   <si>
-    <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
-            &lt;b&gt;What Karvea contains&lt;/b&gt;
-            &lt;ul&gt;
-                &lt;li&gt;The active substance is irbesartan. Each tablet of Karvea 75 mg contains 75 mg irbesartan.&lt;/li&gt;
-                &lt;li&gt;The other ingredients are microcrystalline cellulose, croscarmellose sodium, lactose
-                    monohydrate, magnesium stearate, colloidal hydrated silica, pregelatinised maize starch, and poloxamer 188. Please see section 2 “Karvea contains lactose”.&lt;/li&gt;
-            &lt;/ul&gt;
-            &lt;b&gt;What Karvea looks like and contents of the pack&lt;/b&gt;
-            &lt;p&gt;Karvea 75 mg tablets are white to off-white, biconvex, and oval-shaped with a heart debossed on one side and the number 2771 engraved on the other side.&lt;/p&gt;
-            &lt;p&gt;Karvea 75 mg tablets are supplied in blister packs of 14, 28, 56 or 98 tablets. Unidose blister packs of 56 x 1 tablet for delivery in hospitals are also available.&lt;/p&gt;
-            &lt;p&gt;Not all pack sizes may be marketed.&lt;/p&gt;
-            &lt;b&gt;Marketing Authorisation Holder:&lt;/b&gt;
-            &lt;p&gt;sanofi-aventis groupe&lt;/p&gt;
-            &lt;p&gt;54, rue La Boétie&lt;/p&gt;
-            &lt;p&gt;F-75008 Paris - France&lt;/p&gt;
-            &lt;p&gt;Manufacturer:&lt;/p&gt;
-            &lt;p&gt;SANOFI WINTHROP INDUSTRIE&lt;/p&gt;
-            &lt;p&gt;1, rue de la Vierge&lt;/p&gt;
-            &lt;p&gt;Ambarès and Lagrave&lt;/p&gt;
-            &lt;p&gt;F-33565 Carbon Blanc Cedex - France&lt;/p&gt;
-            &lt;p&gt;SANOFI WINTHROP INDUSTRIE&lt;/p&gt;
-            &lt;p&gt;30-36 Avenue Gustave Eiffel, BP 7166&lt;/p&gt;
-            &lt;p&gt;F-37071 Tours Cedex 2 - France&lt;/p&gt;
-            &lt;p&gt;For any information about this medicinal product, please contact the local representative of the Marketing Authorisation Holder.&lt;/p&gt;
-            &lt;table&gt;
-                &lt;colgroup&gt;
-                    &lt;col /&gt;
-                    &lt;col /&gt;
-                &lt;/colgroup&gt;
-                &lt;thead&gt;
-                    &lt;tr&gt;
-                        &lt;th&gt;&lt;/th&gt;
-                        &lt;th&gt;&lt;/th&gt;
-                    &lt;/tr&gt;
-                &lt;/thead&gt;
-                &lt;tbody&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;België/Belgique/Belgien &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi Belgium&lt;/p&gt;
-                            &lt;p&gt; Tél/Tel: +32 (0)2 710 54 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Lietuva &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma UAB &lt;/p&gt;
-                            &lt;p&gt;Tel: +370 5 236 91 40 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;България &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma EOOD Тел.: +359 (0)2 4942 480 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Luxembourg/Luxemburg &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi Belgium&lt;/p&gt;
-                            &lt;p&gt; Tél/Tel: +32 (0)2 710 54 00 (Belgique/Belgien) &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Česká republika &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis, s.r.o. Tel: +420 233 086 111 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Magyarország &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;SANOFI-A VENTIS Zrt. Tel.: +36 1 505 0050 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Danmark &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi A/S&lt;/p&gt;
-                            &lt;p&gt; Tlf: +45 45 16 70 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Malta &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi S.r.l.&lt;/p&gt;
-                            &lt;p&gt; Tel: +39 02 39394275 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Deutschland &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi-Aventis Deutschland GmbH&lt;/p&gt;
-                            &lt;p&gt; Tel: 0800 52 52 010&lt;/p&gt;
-                            &lt;p&gt; Tel. aus dem Ausland: +49 69 305 21 131 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Norge &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis Norge AS Tlf: +47 67 10 71 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Eesti &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma OÜ Tel: +372 640 10 30 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Österreich &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis GmbH Tel: +43 1 80 185 – 0 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Ελλάδα &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis AEBE Τηλ: +30 210 900 16 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Polska &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis Sp. z o.o. Tel.: +48 22 280 00 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;España &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis, S.A. Tel: +34 93 485 94 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;France &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis France&lt;/p&gt;
-                            &lt;p&gt; Tél: 0 800 222 555&lt;/p&gt;
-                            &lt;p&gt;Appel depuis l’étranger : +33 1 57 63 23 23 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Portugal &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi - Produtos Farmacêuticos, Lda Tel: +351 21 35 89 400 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Hrvatska &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma d.o.o. Tel: +385 1 2078 500 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;România &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi Romania SRL Tel: +40 (0) 21 317 31 36 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Ireland &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis Ireland Ltd. T/A SANOFI Tel: +353 (0) 1 403 56 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Slovenija &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma d.o.o. Tel: +386 1 235 51 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Ísland &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Vistor hf.&lt;/p&gt;
-                            &lt;p&gt; Sími: +354 535 7000 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Slovenská republika &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma s.r.o. Tel: +421 2 208 33 600 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Italia &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi S.r.l. Tel: 800 536389 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Suomi/Finland &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi Oy&lt;/p&gt;
-                            &lt;p&gt; Puh/Tel: +358 (0) 201 200 300 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Κύπρος &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;C.A. Papaellinas Ltd. Τηλ: +357 22 741741 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Sverige &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Sanofi AB&lt;/p&gt;
-                            &lt;p&gt; Tel: +46 (0)8 634 50 00 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;Latvija &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;Swixx Biopharma SIA Tel: +371 6 616 47 50 &lt;/p&gt;
-                        &lt;/td&gt;
-                        &lt;td&gt;
-                            &lt;p&gt;&lt;b&gt;United Kingdom (Northern Ireland) &lt;/b&gt;&lt;/p&gt;
-                            &lt;p&gt;sanofi-aventis Ireland Ltd. T/A SANOFI Tel: +44 (0) 800 035 2525 &lt;/p&gt;
-                        &lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                    &lt;tr&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                        &lt;td&gt;&lt;/td&gt;
-                    &lt;/tr&gt;
-                &lt;/tbody&gt;
-            &lt;/table&gt;
-            &lt;p&gt;This leaflet was last revised in&lt;/p&gt;
-            &lt;p&gt;Detailed information on this medicine is available on the European Medicines Agency web site: http://www.ema.europa.eu/&lt;/p&gt;            
-        &lt;/div&gt;</t>
-  </si>
-  <si>
     <t>languageID</t>
   </si>
   <si>
@@ -806,15 +417,9 @@
     <t>O8232NY3SJ</t>
   </si>
   <si>
-    <t>cc</t>
-  </si>
-  <si>
     <t>Mirtazapine Cinfa</t>
   </si>
   <si>
-    <t>MIRTAZAPINe CINFA 30 mg Coated Tablet</t>
-  </si>
-  <si>
     <t>30 mg</t>
   </si>
   <si>
@@ -849,13 +454,413 @@
   </si>
   <si>
     <t>MIRTAZAPINA CINFA 30 mg Coated Tablet, 30 tablets</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>https://cima.aemps.es/ids</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Lea todo el prospecto detenidamente antes de empezar a tomar este medicamento, porque contiene
+información importante para usted.&lt;/strong&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Conserve este prospecto, ya que puede tener que volver a leerlo.&lt;/li&gt;
+&lt;li&gt;Si tiene alguna duda, consulte a su médico o farmacéutico.&lt;/li&gt;
+&lt;li&gt;Este medicamento se le ha recetado solamente a usted, y no debe dárselo a otras personas aunque tengan
+los mismos síntomas que usted, ya que puede perjudicarles.&lt;/li&gt;
+&lt;li&gt;Si experimenta efectos adversos, consulte a su médico o farmacéutico, incluso si se trata de efectos
+adversos que no aparecen en este prospecto. Ver sección 4. &lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Contenido del prospecto&lt;/p&gt;
+&lt;ol&gt;
+&lt;li&gt;Qué es mirtazapina cinfa y para qué se utiliza&lt;/li&gt;
+&lt;li&gt;Qué necesita saber antes de empezar a tomar mirtazapina cinfa&lt;/li&gt;
+&lt;li&gt;Cómo tomar mirtazapina cinfa&lt;/li&gt;
+&lt;li&gt;Posibles efectos adversos&lt;/li&gt;
+&lt;li&gt;Conservación de mirtazapina cinfa&lt;/li&gt;
+&lt;li&gt;Contenido del envase e información adicional&lt;/li&gt;
+&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;mirtazapina cinfa pertenece al grupo de medicamentos llamados antidepresivos.&lt;/p&gt;
+&lt;p&gt;Mirtazapina se utiliza para tratar la depresión en adultos.&lt;/p&gt;
+&lt;p&gt;Se requieren de 1 a 2 semanas antes de que mirtazapina empiece a hacer efecto. Después de 2 a 4 semanas usted puede empezar a encontrarse mejor. Debe consultar a su médico si empeora o si no mejora después
+de 2 a 4 semanas.&lt;/p&gt;
+&lt;p&gt;Para más información ver la sección 3 &amp;quot;Cuándo puede esperar encontrarse mejor&amp;quot;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;No tome mirtazapina cinfa&lt;/strong&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;si es alérgico a mirtazapina o a alguno de los demás componentes de este medicamento (incluidos
+en la sección 6). En ese caso, consulte a su médico lo antes posible antes de tomar mirtazapina.&lt;/li&gt;
+&lt;li&gt;si está tomando o ha tomado recientemente (en las dos últimas semanas) medicamentos llamados
+inhibidores de la monoaminooxidasa (IMAO).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Advertencias y precauciones&lt;/strong&gt;
+Consulte a su médico o farmacéutico antes de empezar a tomar mirtazapina cinfa&lt;/p&gt;
+&lt;p&gt;NO TOME O CONSULTE A SU MÉDICO ANTES DE EMPEZAR A TOMAR mirtazapina: Si ha sufrido
+alguna vez una erupción cutánea intensa o descamación de la piel, ampollas o llagas en la boca después de
+tomar mirtazapina u otros medicamentos.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Niños y adolescentes&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Mirtazapina no debe utilizarse normalmente en el tratamiento de niños y adolescentes menores de 18 años
+porque no se demostró su eficacia. A la vez, debe saber que en pacientes menores de 18 años existe un
+mayor riesgo de efectos adversos como intentos de suicidio, ideación suicida y hostilidad
+(predominantemente agresión, comportamiento de confrontación e irritación) cuando toman esta clase de
+medicamentos. Pese a ello, el médico puede prescribir mirtazapina a pacientes menores de 18 años cuando
+decida que es lo más conveniente para el paciente. Si el médico ha prescrito mirtazapina a un paciente
+menor de 18 años y desea discutir esta decisión, por favor, vuelva a su médico. Debe informar a su médico
+si aparecen o empeoran alguno de los síntomas que se detallan anteriormente en pacientes menores de 18
+años que están tomando mirtazapina. Además, todavía no se conocen los efectos sobre la seguridad a largo
+plazo relacionados con el crecimiento, la madurez y el desarrollo del conocimiento y la conducta de
+mirtazapina en este grupo de edad. También se ha observado con mayor frecuencia un considerable
+aumento de peso en este grupo de edad cuando son tratados con mirtazapina, en comparación con los
+adultos.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Ideas de suicidio y empeoramiento de la depresión&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Si se encuentra deprimido puede que a veces tenga ideas de hacerse daño a si mismo o de suicidarse. Esto
+podría empeorar cuando empieza a tomar los antidepresivos por primera vez, ya que estos medicamentos
+tardan en hacer efecto normalmente dos semanas o a veces más.
+Podría ser más propenso a pensar de esta manera:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;si previamente ha tenido pensamientos suicidas o de hacerse daño a si mismo.&lt;/li&gt;
+&lt;li&gt;si es un adulto joven. La información de los ensayos clínicos ha mostrado un riesgo aumentado de
+comportamiento suicida en adultos menores de 25 años con trastornos psiquiátricos y que estaban
+en tratamiento con un antidepresivo.&lt;/li&gt;
+&lt;li&gt;si tiene pensamiento de hacerse daño a si mismo o suicidarse en algún momento, consulte a su
+médico o vaya a un hospital inmediatamente.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Puede ser útil decirle a un pariente o amigo cercano que se encuentra deprimido, y pedirle que lea este
+prospecto. Puede pedirle que le diga si cree que su depresión está empeorando, o si está preocupado por
+cambios en su comportamiento.&lt;/p&gt;
+&lt;p&gt;Asimismo, tenga especial cuidado con mirtazapina:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;si tiene o ha tenido alguna vez uno de los siguientes trastornos&lt;/li&gt;
+&lt;li&gt;Informe a su médico sobre estas situaciones antes de tomar mirtazapina, si no lo ha hecho ya:&lt;ul&gt;
+&lt;li&gt;convulsiones (epilepsia). Si aparecen convulsiones o sus convulsiones son más frecuentes, deje
+de tomar mirtazapina y contacte con su médico inmediatamente;&lt;/li&gt;
+&lt;li&gt;enfermedades del hígado, incluyendo ictericia. Si aparece ictericia, deje de tomar mirtazapina
+y contacte con su médico inmediatamente;&lt;/li&gt;
+&lt;li&gt;enfermedades de los riñones;&lt;/li&gt;
+&lt;li&gt;enfermedad del corazón o presión arterial baja;&lt;/li&gt;
+&lt;li&gt;esquizofrenia. Si los síntomas psicóticos, como los pensamientos paranoicos, son más
+frecuentes o graves contacte con su médico inmediatamente;&lt;/li&gt;
+&lt;li&gt;depresión bipolar (se alternan períodos de animación/hiperactividad y períodos de depresión).
+Si empieza a sentirse animado o sobreexcitado, deje de tomar mirtazapina y contacte con su
+médico inmediatamente;&lt;/li&gt;
+&lt;li&gt;diabetes (podría necesitar ajustar su dosis de insulina u otros medicamentos antidiabéticos);&lt;/li&gt;
+&lt;li&gt;enfermedades de los ojos, como aumento de la presión en el ojo (glaucoma);&lt;/li&gt;
+&lt;li&gt;dificultades para orinar, que podrían deberse a un aumento del tamaño de la próstata;&lt;/li&gt;
+&lt;li&gt;ciertos tipos de enfermedades del corazón que pueden cambiar el ritmo de su corazón, un
+ataque reciente al corazón, un fallo del corazón, o toma de ciertos medicamentos que pueden
+afectar el ritmo del corazón.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;si aparecen signos de infección como fiebre alta inexplicable, dolor de garganta y llagas en la boca
+Deje de tomar mirtazapina y contacte con su médico inmediatamente para realizar un análisis de
+sangre.
+En raras ocasiones, estos síntomas pueden ser signos de alteraciones en la producción de células
+sanguíneas en la médula ósea. Aunque raros, estos síntomas aparecen a las 4-6 semanas de
+tratamiento.&lt;/li&gt;
+&lt;li&gt;si es una persona mayor podría ser más sensible a los efectos adversos de los medicamentos
+antidepresivos.&lt;/li&gt;
+&lt;li&gt;se han notificado con el uso de mirtazapina reacciones cutáneas graves, como síndrome de StevensJohnson (SSJ), necrólisis epidérmica tóxica (NET) y reacción medicamentosa con eosinofilia y
+síntomas sistémicos (DRESS). Interrumpa su uso y busque atención médica inmediatamente si nota
+alguno de los síntomas descritos en la sección 4 en relación con estas reacciones cutáneas graves.
+Si ha sufrido alguna vez reacciones cutáneas graves, no debe reiniciarse el tratamiento con
+mirtazapina.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Otros medicamentos y mirtazapina cinfa&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Informe a su médico o farmacéutico si está tomando, ha tomado recientemente o pudiera tener que tomar
+cualquier otro medicamento.&lt;/p&gt;
+&lt;p&gt;No tome mirtazapina junto con:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;inhibidores de la monoamino oxidasa (inhibidores de la MAO). Asimismo, no tome mirtazapina
+durante las dos semanas después de haber dejado de tomar los inhibidores de la MAO. Si deja de
+tomar mirtazapina, tampoco tome inhibidores de la MAO durante las siguientes dos semanas.
+Ejemplos de inhibidores de la MAO son moclobemida, tranilcipromina (ambos son antidepresivos)
+y selegilina (para la enfermedad de Parkinson).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Tenga cuidado si toma mirtazapina junto con:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;antidepresivos como los inhibidores selectivos de la recaptación de serotonina (ISRSs),
+venlafaxina y L-triptófano o triptanos (utilizados para tratar la migraña), tramadol (para el
+dolor), linezolid (un antibiótico), litio (utilizado para tratar algunos trastornos psiquiátricos), azul
+de metileno (utilizado para tratar niveles altos de metahemoglobina en la sangre) y preparados a
+base de Hierba de San Juan – Hypericum perforatum (planta medicinal para la depresión). En
+casos muy raros, mirtazapina solo o junto con estos medicamentos, puede dar lugar al llamado
+síndrome serotoninérgico. Algunos de los síntomas de este síndrome son: fiebre inexplicable,
+sudoración, palpitaciones, diarrea, contracciones musculares (incontrolables), escalofríos, reflejos
+exagerados, agitación, cambios de humor y pérdida de conciencia. Si presenta una combinación de
+estos síntomas, consulte a su médico inmediatamente.&lt;/li&gt;
+&lt;li&gt;el antidepresivo nefazodona. Puede aumentar la cantidad de mirtazapina en sangre. Informe a su
+médico si está tomando este medicamento. Podría ser necesario disminuir la dosis de mirtazapina, o
+aumentarla nuevamente al dejar de tomar nefazodona.&lt;/li&gt;
+&lt;li&gt;medicamentos para la ansiedad o el insomnio como las benzodiazepinas.
+medicamentos para la esquizofrenia como la olanzapina.
+medicamentos para las alergias como la cetirizina.
+medicamentos para el dolor intenso como la morfina.
+En combinación con estos medicamentos, mirtazapina puede aumentar la somnolencia causada por
+estos medicamentos.&lt;/li&gt;
+&lt;li&gt;medicamentos para infecciones: medicamentos para infecciones bacterianas (como la
+eritromicina), medicamentos para infecciones por hongos (como el ketoconazol) y los
+medicamentos para el VIH/SIDA (inhibidores de la proteasa del VIH) y medicamentos para la
+úlcera de estómago (como la cimetidina). Si se toman junto con mirtazapina, estos medicamentos
+pueden aumentar la cantidad de mirtazapina en sangre. Informe a su médico si está tomando estos
+medicamentos. Podría ser necesario disminuir la dosis de mirtazapina, o aumentarla nuevamente al
+dejar de tomar estos medicamentos.&lt;/li&gt;
+&lt;li&gt;medicamentos para la epilepsia: como la carbamazepina y la fenitoína.&lt;/li&gt;
+&lt;li&gt;medicamentos para la tuberculosis como la rifampicina.
+Si se toman junto con mirtazapina, estos medicamentos pueden reducir la cantidad de mirtazapina
+en sangre. Informe a su médico si está tomando estos medicamentos. Podría ser necesario aumentar
+la dosis de mirtazapina, o disminuirla nuevamente al dejar de tomar estos medicamentos.
+medicamentos para prevenir la coagulación de la sangre como la warfarina. Mirtazapina puede
+aumentar los efectos de la warfarina en la sangre. Informe a su médico si está tomando este
+medicamento. En caso de tomarlos a la vez, se recomienda que el médico le haga controles en
+sangre.&lt;/li&gt;
+&lt;li&gt;medicamentos que pueden afectar el ritmo del corazón, como ciertos antibióticos y algunos
+antipsicóticos&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Toma de mirtazapina cinfa con alimentos y alcohol&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Puede sentirse somnoliento si bebe alcohol mientras esté en tratamiento con mirtazapina. Se recomienda no
+beber nada de alcohol.
+Puede tomar mirtazapina con o sin alimentos.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Embarazo y lactancia&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Si está embarazada o en periodo de lactancia, cree que podría estar embarazada o tiene intención de
+quedarse embarazada, consulte a su médico o farmacéutico antes de utilizar este medicamento.&lt;/p&gt;
+&lt;p&gt;La experiencia limitada de la administración de mirtazapina a mujeres embarazadas no indica un aumento
+de riesgo. Sin embargo, debe tenerse cuidado si se usa durante el embarazo.&lt;/p&gt;
+&lt;p&gt;Si usa mirtazapina hasta, o poco antes del parto, su hijo será examinado para detectar posibles efectos
+adversos.&lt;/p&gt;
+&lt;p&gt;Tomados durante el embarazo, los medicamentos similares (ISRS) pueden aumentar en los bebés el riesgo
+de padecer una enfermedad grave denominada hipertensión pulmonar persistente neonatal (HPPN),
+ocasionando que el bebé respire más rápido y adquiera un tono azulado. Estos síntomas comienzan
+normalmente durante las primeras 24 horas después de que nazca el bebé. Si esto le sucede al bebé, debe
+consultar a su matrona o médico de inmediato.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Conducción y uso de máquinas&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Durante el tratamiento con mirtazapina puede que se sienta 
+somnoliento o mareado. No conduzca ni
+maneje herramientas o máquinas hasta que sepa cómo le afecta el tratamiento con mirtazapina.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;mirtazapina cinfa contiene lactosa.&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Este medicamento contiene lactosa. Si su médico le ha indicado que padece una intolerancia a ciertos
+azúcares, consulte con él antes de tomar este medicamento.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Siga exactamente las instrucciones de administración de este medicamento indicadas por su médico o
+farmacéutico. En caso de duda, consulte de nuevo a su médico o farmacéutico.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Cuánto tomar&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;La dosis inicial recomendada es de 15 o 30 mg al día. Su médico puede recomendarle aumentar la dosis
+tras unos días hasta la cantidad que sea mejor para usted (entre 15 y 45 mg al día). Normalmente la dosis es
+la misma para todas las edades. Sin embargo, si es una persona mayor o si padece una enfermedad del
+riñón o del hígado, su médico podría cambiar la dosis.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Cuándo tomar mirtazapina&lt;/strong&gt; &lt;/p&gt;
+&lt;p&gt;Tome mirtazapina a la misma hora cada día.
+Es mejor tomar la dosis de mirtazapina de una sola vez antes de acostarse. Sin embargo, su médico puede
+recomendarle que divida su dosis de mirtazapina por la mañana y por la noche antes de acostarse. La dosis
+más alta debe tomarse antes de acostarse.
+Los comprimidos se toman por vía oral. Tome la dosis de mirtazapina recetada sin masticar, con agua o
+zumo.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Cuándo puede esperar encontrarse mejor&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Normalmente mirtazapina empezará a hacer efecto después de 1 o 2 semanas y después de 2 a 4 semanas
+podría empezar a encontrarse mejor.
+Es importante que durante las primeras semanas de tratamiento hable con su médico sobre los efectos de
+mirtazapina: entre 2 y 4 semanas después de haber empezado a tomar mirtazapina, hable con su médico
+sobre cómo le ha afectado este medicamento.
+Si todavía no se encuentra mejor, su médico podría recetarle una dosis mayor. En ese caso, hable
+nuevamente con su médico después de otras 2-4 semanas.
+Normalmente necesitará tomar mirtazapina hasta que los síntomas de depresión hayan desaparecido
+durante 4-6 meses.&lt;/p&gt;
+&lt;p&gt;El comprimido se puede partir en dosis iguales.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Si toma más mirtazapina cinfa del que debe&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;En caso de sobredosis o ingestión accidental consulte inmediatamente a su médico o farmacéutico o llame
+al Servicio de Información Toxicológica, teléfono 91 562 04 20, indicando el medicamento y la cantidad
+ingerida. Se recomienda llevar el prospecto y el envase al profesional sanitario.&lt;/p&gt;
+&lt;p&gt;Los síntomas más probables de una sobredosis de mirtazapina (sin otros medicamentos o alcohol) son la
+somnolencia, desorientación y palpitaciones. Los síntomas de una posible sobredosis pueden incluir
+cambios en el ritmo de su corazón (latido rápido, irregular) y/o desfallecimiento, que podrían ser síntomas
+de una enfermedad potencialmente mortal conocida como Torsades de pointes.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Si olvidó tomar mirtazapina cinfa&lt;/strong&gt; &lt;/p&gt;
+&lt;p&gt;Si tiene que tomar su dosis una vez al día&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;No tome una dosis doble para compensar las dosis olvidadas. 
+Tome la dosis habitual al día siguiente.
+Si tiene que tomar su dosis dos veces al día&lt;/li&gt;
+&lt;li&gt;Si ha olvidado la dosis de la mañana, simplemente tómesela junto con la dosis de la noche.&lt;/li&gt;
+&lt;li&gt;Si ha olvidado la dosis de la noche, no la tome a la mañana siguiente; sáltesela y continúe con sus
+dosis normales por la mañana y por la noche.&lt;/li&gt;
+&lt;li&gt;Si ha olvidado ambas dosis, no intente recuperarlas. Sáltese ambas dosis y al día siguiente continúe
+con la dosis normal por la mañana y por la noche.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Si interrumpe el tratamiento con mirtazapina cinfa&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Deje de tomar mirtazapina sólo si lo consulta con su médico.
+Si lo deja demasiado pronto, la depresión podría reaparecer. Cuando se encuentre mejor, hable con su
+médico. Su médico decidirá cuándo puede dejar el tratamiento.
+No deje de tomar mirtazapina bruscamente, aun cuando la depresión haya desaparecido. Si deja de tomar
+mirtazapina de forma brusca, puede sentirse enfermo, mareado, agitado o ansioso y tener dolores de
+cabeza. Estos síntomas pueden evitarse dejando el tratamiento gradualmente. Su médico le indicará cómo
+disminuir la dosis gradualmente.&lt;/p&gt;
+&lt;p&gt;Si tiene cualquier otra duda sobre el uso de este medicamento, pregunte a su médico o farmacéutico.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Al igual que todos los medicamentos, este medicamento puede producir efectos adversos, aunque no todas
+las personas los sufran.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Si experimenta alguno de los siguientes efectos adversos graves, deje de tomar mirtazapina e informe inmediatamente a su médico.&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Poco frecuentes (pueden afectar hasta 1 de cada 100 pacientes):&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;sentimiento de euforia exagerada (manía).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Raros (pueden afectar hasta 1 de cada 1.000 pacientes):&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;coloración amarilla de los ojos o la piel; puede sugerir alteraciones en el funcionamiento del hígado
+(ictericia).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Frecuencia no conocida (no puede estimarse a partir de los datos disponibles):&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;signos de infección tales como fiebre alta inexplicable y repentina, dolor de garganta y llagas en la boca
+(agranulocitosis). En casos raros, mirtazapina puede provocar alteraciones en la producción de células
+sanguíneas (depresión de la médula ósea). Algunas personas se vuelven menos resistentes a las
+infecciones porque mirtazapina puede provocar una disminución temporal de los glóbulos blancos de la
+sangre (granulocitopenia). En casos raros, mirtazapina también puede provocar una disminución de los
+glóbulos rojos y blancos y de las plaquetas (anemia aplásica), una disminución de las plaquetas
+(trombocitopenia) o un aumento en el número de glóbulos blancos en sangre (eosinofilia).&lt;/li&gt;
+&lt;li&gt;ataque epiléptico (convulsiones).&lt;/li&gt;
+&lt;li&gt;combinación de síntomas como fiebre inexplicable, sudoración, palpitaciones, diarrea, contracciones
+musculares (incontrolables), escalofríos, reflejos exagerados, agitación, cambios de humor, pérdida de
+conciencia y aumento de la producción de saliva. En casos muy raros, estos síntomas pueden ser señales
+de un trastorno llamado “síndrome serotoninérgico”.&lt;/li&gt;
+&lt;li&gt;pensamientos de hacerse daño a uno mismo o de suicidio.&lt;/li&gt;
+&lt;li&gt;reacciones graves en la piel:&lt;ul&gt;
+&lt;li&gt;parches rojos en el tronco, como máculas circunscritas o circulares, a menudo con ampollas en el
+centro, desprendimiento de la piel, úlceras en la boca, la garganta, la nariz, los genitales y los ojos.
+Estos eritemas cutáneos graves pueden ir precedidos de fiebre y síntomas gripales (síndrome de
+Stevens-Johnson, necrólisis epidérmica tóxica).&lt;/li&gt;
+&lt;li&gt;eritema generalizado, temperatura corporal elevada y aumento de tamaño de los ganglios linfáticos
+(síndrome DRESS o síndrome de hipersensibilidad medicamentosa).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Otros posibles efectos adversos con mirtazapina son:&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Muy frecuentes (pueden afectar a más de 1 de cada 10 pacientes)&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;aumento del apetito y aumento de peso&lt;/li&gt;
+&lt;li&gt;somnolencia&lt;/li&gt;
+&lt;li&gt;dolor de cabeza&lt;/li&gt;
+&lt;li&gt;boca seca&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Frecuentes (pueden afectar hasta 1 de cada 10 pacientes)&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;letargia&lt;/li&gt;
+&lt;li&gt;mareo&lt;/li&gt;
+&lt;li&gt;temblor&lt;/li&gt;
+&lt;li&gt;náuseas&lt;/li&gt;
+&lt;li&gt;diarrea&lt;/li&gt;
+&lt;li&gt;vómitos&lt;/li&gt;
+&lt;li&gt;estreñimiento&lt;/li&gt;
+&lt;li&gt;urticaria o erupciones en la piel (exantema)&lt;/li&gt;
+&lt;li&gt;dolores en las articulaciones (artralgia) o músculos (mialgia)&lt;/li&gt;
+&lt;li&gt;dolor de espalda&lt;/li&gt;
+&lt;li&gt;mareo o desmayo al levantarse rápidamente (hipotensión ortrtostática)&lt;/li&gt;
+&lt;li&gt;hinchazón (normalmente en tobillos o pies) debido a retención de líquidos (edema)&lt;/li&gt;
+&lt;li&gt;cansancio&lt;/li&gt;
+&lt;li&gt;sueños vívidos&lt;/li&gt;
+&lt;li&gt;confusión&lt;/li&gt;
+&lt;li&gt;ansiedad&lt;/li&gt;
+&lt;li&gt;dificultades para dormir&lt;/li&gt;
+&lt;li&gt;problemas de memoria, que en la mayoría de los casos se resolvieron cuando se suspendió el
+tratamiento&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Poco frecuentes (pueden afectar hasta 1 de cada 100 pacientes)&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;sensación extraña en la piel por ejemplo quemazón, pinchazos, cosquilleo u hormigueo (parestesia)&lt;/li&gt;
+&lt;li&gt;movimientos involuntarios de agitación de las piernas durante el sueño&lt;/li&gt;
+&lt;li&gt;desmayos (síncope)&lt;/li&gt;
+&lt;li&gt;sensación de adormecimiento de la boca (hipoestesia oral)&lt;/li&gt;
+&lt;li&gt;tensión baja&lt;/li&gt;
+&lt;li&gt;pesadillas&lt;/li&gt;
+&lt;li&gt;agitación&lt;/li&gt;
+&lt;li&gt;alucinaciones&lt;/li&gt;
+&lt;li&gt;incapacidad para mantenerse quieto&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Raros (pueden afectar hasta 1 de cada 1.000 pacientes)&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;tics o contracciones musculares (mioclono)&lt;/li&gt;
+&lt;li&gt;agresión&lt;/li&gt;
+&lt;li&gt;dolor abdominal, náuseas; esto puede indicar inflamación del páncreas (pancreatitis)&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Frecuencia no conocida (no puede estimarse a partir de los datos disponibles)&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;sensaciones anormales en la boca (parestesia oral)&lt;/li&gt;
+&lt;li&gt;hinchazón en la boca (edema bucal)&lt;/li&gt;
+&lt;li&gt;hinchazón por todo el cuerpo (edema generalizado)&lt;/li&gt;
+&lt;li&gt;hinchazón localizada&lt;/li&gt;
+&lt;li&gt;hiponatremia&lt;/li&gt;
+&lt;li&gt;secreción inadecuada de hormona antidiurética&lt;/li&gt;
+&lt;li&gt;reacciones graves en la piel (dermatitis bullosa, eritema multiforme)&lt;/li&gt;
+&lt;li&gt;andar dormido (sonambulismo)&lt;/li&gt;
+&lt;li&gt;problema del habla&lt;/li&gt;
+&lt;li&gt;aumento de los niveles de creatina cinasa en la sangre&lt;/li&gt;
+&lt;li&gt;dificultad para orinar (retención urinaria)&lt;/li&gt;
+&lt;li&gt;dolor muscular, rigidez y/o debilidad, oscurecimiento o decoloración de la orina (rabdomiólisis)&lt;/li&gt;
+&lt;li&gt;aumento de los niveles de la hormona prolactina en la sangre (hiperprolactinemia, que incluye
+síntomas de aumento de tamaño de las mamas y/o secreción lechosa por el pezón) &lt;/li&gt;
+&lt;li&gt;erección dolorosa y prolongada del pene&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Otros efectos adversos en niños y adolescentes&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;En menores de 18 años se observaron frecuentemente los siguientes efectos adversos en los ensayos
+clínicos: un considerable aumento de peso, urticaria y un aumento de triglicéridos en la sangre.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Comunicación de efectos adversos&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Si experimenta cualquier tipo de efecto adverso, consulte a su médico o farmacéutico, incluso si se trata de
+posibles efectos adversos que no aparecen en este prospecto. También puede comunicarlos directamente a
+través del Sistema Español de Farmacovigilancia de Medicamentos de Uso Humano:
+&lt;a href="https://www.notificaram.es"&gt;https://www.notificaram.es&lt;/a&gt;. Mediante la comunicación de efectos adversos usted puede contribuir a
+proporcionar más información sobre la seguridad de este medicamento.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mantener este medicamento fuera de la vista y del alcance de los niños.&lt;/p&gt;
+&lt;p&gt;No utilice este medicamento después de la fecha de caducidad que aparece en el envase y en el blíster,
+después de CAD. La fecha de caducidad es el último día del mes que se indica.&lt;/p&gt;
+&lt;p&gt;No conservar a temperatura superior a 30ºC.&lt;/p&gt;
+&lt;p&gt;Los medicamentos no se deben tirar por los desagües ni a la basura. Deposite los envases y los
+medicamentos que no necesita en el Punto SIGRE de la farmacia. En caso de duda, pregunte a su
+farmacéutico cómo deshacerse de los envases y de los medicamentos que ya no necesita. De esta forma,
+ayudará a proteger el medio ambiente.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Composición de mirtazapina cinfa&lt;/strong&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;El principio activo es mirtazapina. Cada comprimido recubierto con película contiene 30 mg de
+mirtazapina.&lt;/li&gt;
+&lt;li&gt;Los demás componentes son:&lt;ul&gt;
+&lt;li&gt;Núcleo del comprimido: lactosa monohidrato, hidroxipropilcelulosa (E-463), almidón de maíz,
+sílice coloidal anhidra, hidroxipropilcelulosa de bajo grado de sustitución (E-463) y estearato de
+magnesio.&lt;/li&gt;
+&lt;li&gt;Recubrimiento del comprimido: Opadry Brown 20A56788 (hidroxipropilcelulosa (E-463),
+hipromelosa (E-464), dióxido de titanio (E-171), óxido de hierro amarillo (E-172), óxido de hierro
+rojo (E-172) y óxido de hierro negro (E-172)).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Aspecto del producto y contenido del envase&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;Comprimidos de color marrón rojizo, biconvexos, con forma de cápsula, recubiertos, ranurados por una
+cara y marcados con el código “30” por la otra cara.&lt;/p&gt;
+&lt;p&gt;Se presenta en blísteres de PVC-PVDC/ALU.&lt;/p&gt;
+&lt;p&gt;Cada envase contiene 30 o 500 (envase clínico) comprimidos recubiertos con película.&lt;/p&gt;
+&lt;p&gt;Puede que solamente estén comercializados algunos tamaños de envases.&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Titular de la autorización de comercialización y responsable de la fabricación&lt;/strong&gt; &lt;/p&gt;
+&lt;p&gt;Laboratorios Cinfa, S.A.  &lt;/p&gt;
+&lt;p&gt;Carretera Olaz-Chipi, 10. Polígono Industrial Areta  &lt;/p&gt;
+&lt;p&gt;31620 Huarte (Navarra) - España  &lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Fecha de la última revisión de este prospecto: Noviembre 2021&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;La información detallada y actualizada de este medicamento está disponible en la página web de la Agencia
+Española de Medicamentos y Productos Sanitarios (AEMPS) www.aemps.gob.es/&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -953,6 +958,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC3E88D"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -975,7 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -998,6 +1009,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -1359,7 +1371,7 @@
         <v>71</v>
       </c>
       <c r="L1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="M1" t="s">
         <v>10</v>
@@ -1368,10 +1380,10 @@
     <row r="2" spans="1:13" ht="19">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -1389,13 +1401,13 @@
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="L2" s="13">
         <v>31620</v>
@@ -1412,7 +1424,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1450,25 +1462,25 @@
         <v>84</v>
       </c>
       <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>91</v>
       </c>
-      <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N1" t="s">
-        <v>97</v>
-      </c>
       <c r="O1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="P1" t="s">
         <v>10</v>
@@ -1477,7 +1489,7 @@
     <row r="2" spans="1:16" ht="409.6">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>56</v>
@@ -1489,32 +1501,32 @@
         <v>59</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I2" t="s">
-        <v>88</v>
+      <c r="H2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1528,7 +1540,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1568,7 +1580,7 @@
         <v>44910</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1624,10 +1636,10 @@
     <row r="2" spans="1:11">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
@@ -1636,7 +1648,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
@@ -1645,10 +1657,10 @@
         <v>100000072062</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1723,10 +1735,10 @@
     <row r="2" spans="1:14" ht="21">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -1735,16 +1747,16 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H2" t="s">
         <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K2" t="s">
         <v>45</v>
@@ -1828,10 +1840,10 @@
     <row r="2" spans="1:13" ht="21">
       <c r="A2" s="1"/>
       <c r="B2" s="11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1848,10 +1860,10 @@
     <row r="3" spans="1:13" ht="21">
       <c r="A3" s="1"/>
       <c r="B3" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1868,10 +1880,10 @@
     <row r="4" spans="1:13" ht="21">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1898,10 +1910,10 @@
     <row r="5" spans="1:13" ht="21">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1918,7 +1930,7 @@
     <row r="6" spans="1:13" ht="21">
       <c r="A6" s="1"/>
       <c r="B6" s="11" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>20</v>
@@ -1938,10 +1950,10 @@
     <row r="7" spans="1:13" ht="21">
       <c r="A7" s="1"/>
       <c r="B7" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -1999,28 +2011,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EB2795-F6E7-D149-BA96-099EC7B435E4}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2028,85 +2040,94 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" t="s">
-        <v>103</v>
-      </c>
       <c r="N1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="O1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="P1" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" t="s">
-        <v>132</v>
+        <v>100</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="E2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" t="s">
-        <v>121</v>
-      </c>
       <c r="J2" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
-        <v>102</v>
-      </c>
-      <c r="L2" s="9">
+      <c r="L2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="9">
         <v>100000000000</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B86962CD-3E6E-3B4E-A8C4-596368C5CEA4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2117,7 +2138,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2158,7 +2179,7 @@
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>83</v>
@@ -2167,7 +2188,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F2" s="14">
         <v>100000073380</v>
@@ -2242,7 +2263,7 @@
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2251,7 +2272,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F2" s="14">
         <v>100000073380</v>
@@ -2339,7 +2360,7 @@
         <v>74</v>
       </c>
       <c r="L1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M1" t="s">
         <v>35</v>
@@ -2351,25 +2372,25 @@
         <v>40</v>
       </c>
       <c r="P1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="Q1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="R1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="S1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="T1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="U1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="V1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="W1" t="s">
         <v>10</v>
@@ -2378,7 +2399,7 @@
     <row r="2" spans="1:23">
       <c r="A2" s="1"/>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
@@ -2393,7 +2414,7 @@
         <v>100000155527</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I2">
         <v>123456</v>
@@ -2425,7 +2446,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>